<commit_message>
Tradução da história principal
</commit_message>
<xml_diff>
--- a/Excel/bootpar/boot/tips_tutorial.xlsx
+++ b/Excel/bootpar/boot/tips_tutorial.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
   <si>
     <t>COLUMNA</t>
   </si>
@@ -611,9 +611,15 @@
     <t>View the &lt;Color:255, 200, 200, 255&gt;Notebook&lt;Color:Default&gt; from the Pause Menu by pressing the\n&lt;Sign:21&gt;. More items are added to the &lt;Color:255, 200, 200, 255&gt;Notebook&lt;Color:Default&gt; as\nthe story progresses and you discover more tips on the way.\n\nThis guide contains a wide range of useful information.\nWhenever you need some help, look through the Notebook!</t>
   </si>
   <si>
+    <t>Veja as &lt;Cor:255, 200, 200, 255&gt;Notas&lt;Cor:Default&gt; no Menu pressionando\n&lt;Sign:21&gt;. Mais itens são adicionados as &lt;Cor:255, 200, 200, 255&gt;Notas&lt;Cor:Default&gt; à medida que a história avança e você descobre mais dicas sobre o caminho.\n\nEste guia contém uma grande variedade de informações úteis.\nQuando você precisar de ajuda, olhe as Notas!</t>
+  </si>
+  <si>
     <t>The game can be saved from the Pause Menu or wherever the\nsave point icon appears, such as at telephone booths or\nat an accessible hideout.\n\nSaving records the current game status, so you can continue\nfrom the same point in a save file when the game is resumed.</t>
   </si>
   <si>
+    <t>O jogo pode ser salvo no Menu ou em locais que o ícone de gravação apareça, como por exemplo em cabines telefônicas ou em um esconderijo acessível.\n\nSe salvar o status do jogo atual, você pode continuar a jogar a partir daquele mesmo ponto caso o jogo seja reiniciado.</t>
+  </si>
+  <si>
     <t>In certain situations words such as "Talk" or "Exit" will\nappear at the top-right corner, along with a button icon.\nThese contextual prompts are called Action Icons.\n\nPress the indicated button to perform the action displayed.</t>
   </si>
   <si>
@@ -1077,6 +1083,9 @@
   </si>
   <si>
     <t>You can save from the Pause Menu\nor at phones and hideouts.</t>
+  </si>
+  <si>
+    <t>Você pode salvar no Menu ou em telefones e esconderijos.</t>
   </si>
   <si>
     <t>Press the button shown when prompts such\nas "Talk" appear to perform that action.</t>
@@ -2877,7 +2886,7 @@
         <v>198</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="112">
@@ -2888,10 +2897,10 @@
         <v>2</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113">
@@ -2902,10 +2911,10 @@
         <v>3</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="114">
@@ -2916,10 +2925,10 @@
         <v>4</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="115">
@@ -2930,10 +2939,10 @@
         <v>5</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="116">
@@ -2944,10 +2953,10 @@
         <v>6</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="117">
@@ -2958,10 +2967,10 @@
         <v>7</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="118">
@@ -2972,10 +2981,10 @@
         <v>8</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="119">
@@ -2986,10 +2995,10 @@
         <v>9</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120">
@@ -3000,10 +3009,10 @@
         <v>10</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121">
@@ -3014,10 +3023,10 @@
         <v>11</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="122">
@@ -3028,10 +3037,10 @@
         <v>12</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="123">
@@ -3042,10 +3051,10 @@
         <v>13</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="124">
@@ -3056,10 +3065,10 @@
         <v>14</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="125">
@@ -3070,10 +3079,10 @@
         <v>15</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="126">
@@ -3084,10 +3093,10 @@
         <v>16</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127">
@@ -3098,10 +3107,10 @@
         <v>17</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="128">
@@ -3112,10 +3121,10 @@
         <v>18</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="129">
@@ -3126,10 +3135,10 @@
         <v>19</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="130">
@@ -3140,10 +3149,10 @@
         <v>20</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="131">
@@ -3154,10 +3163,10 @@
         <v>21</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="132">
@@ -3168,10 +3177,10 @@
         <v>22</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="133">
@@ -3182,10 +3191,10 @@
         <v>23</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="134">
@@ -3196,10 +3205,10 @@
         <v>24</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="135">
@@ -3210,10 +3219,10 @@
         <v>25</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="136">
@@ -3224,10 +3233,10 @@
         <v>26</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="137">
@@ -3238,10 +3247,10 @@
         <v>27</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="138">
@@ -3252,10 +3261,10 @@
         <v>28</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="139">
@@ -3266,10 +3275,10 @@
         <v>29</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="140">
@@ -3280,10 +3289,10 @@
         <v>30</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="141">
@@ -3294,10 +3303,10 @@
         <v>31</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="142">
@@ -3308,10 +3317,10 @@
         <v>32</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="143">
@@ -3322,10 +3331,10 @@
         <v>33</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="144">
@@ -3336,10 +3345,10 @@
         <v>34</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="145">
@@ -3350,10 +3359,10 @@
         <v>35</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="146">
@@ -3364,10 +3373,10 @@
         <v>36</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="147">
@@ -3378,10 +3387,10 @@
         <v>37</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="148">
@@ -3392,10 +3401,10 @@
         <v>38</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="149">
@@ -3406,10 +3415,10 @@
         <v>39</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D149" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="150">
@@ -3420,10 +3429,10 @@
         <v>40</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="151">
@@ -3434,10 +3443,10 @@
         <v>41</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="152">
@@ -3448,10 +3457,10 @@
         <v>42</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="153">
@@ -3462,10 +3471,10 @@
         <v>43</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="154">
@@ -3476,10 +3485,10 @@
         <v>44</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="155">
@@ -3490,10 +3499,10 @@
         <v>45</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="156">
@@ -3504,10 +3513,10 @@
         <v>46</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="157">
@@ -3518,10 +3527,10 @@
         <v>47</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="158">
@@ -3532,10 +3541,10 @@
         <v>48</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="159">
@@ -3546,10 +3555,10 @@
         <v>49</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="160">
@@ -3560,10 +3569,10 @@
         <v>50</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="161">
@@ -3574,10 +3583,10 @@
         <v>51</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D161" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="162">
@@ -3588,10 +3597,10 @@
         <v>52</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="163">
@@ -3602,10 +3611,10 @@
         <v>53</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="164">
@@ -3616,10 +3625,10 @@
         <v>54</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="165">
@@ -3630,10 +3639,10 @@
         <v>55</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="166">
@@ -3644,10 +3653,10 @@
         <v>56</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="167">
@@ -3658,10 +3667,10 @@
         <v>57</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="168">
@@ -3672,10 +3681,10 @@
         <v>58</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="169">
@@ -3686,10 +3695,10 @@
         <v>59</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="170">
@@ -3700,10 +3709,10 @@
         <v>60</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="171">
@@ -3714,10 +3723,10 @@
         <v>61</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="172">
@@ -3728,10 +3737,10 @@
         <v>62</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="173">
@@ -3742,10 +3751,10 @@
         <v>63</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="174">
@@ -3756,10 +3765,10 @@
         <v>64</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="175">
@@ -3770,10 +3779,10 @@
         <v>65</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="176">
@@ -3784,10 +3793,10 @@
         <v>66</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D176" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="177">
@@ -3798,10 +3807,10 @@
         <v>67</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="178">
@@ -3812,10 +3821,10 @@
         <v>68</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="179">
@@ -3826,10 +3835,10 @@
         <v>69</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D179" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="180">
@@ -3840,10 +3849,10 @@
         <v>70</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="181">
@@ -3854,10 +3863,10 @@
         <v>71</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="182">
@@ -3868,10 +3877,10 @@
         <v>72</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="183">
@@ -3882,10 +3891,10 @@
         <v>73</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="184">
@@ -3896,10 +3905,10 @@
         <v>74</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="185">
@@ -3910,10 +3919,10 @@
         <v>75</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="186">
@@ -3924,10 +3933,10 @@
         <v>76</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="187">
@@ -3938,10 +3947,10 @@
         <v>77</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="188">
@@ -3952,10 +3961,10 @@
         <v>78</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D188" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="189">
@@ -3966,10 +3975,10 @@
         <v>79</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D189" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="190">
@@ -3980,10 +3989,10 @@
         <v>80</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="191">
@@ -3994,10 +4003,10 @@
         <v>81</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="192">
@@ -4008,10 +4017,10 @@
         <v>82</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="193">
@@ -4022,10 +4031,10 @@
         <v>83</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="194">
@@ -4036,10 +4045,10 @@
         <v>84</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="195">
@@ -4050,10 +4059,10 @@
         <v>85</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="196">
@@ -4064,10 +4073,10 @@
         <v>86</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="197">
@@ -4078,10 +4087,10 @@
         <v>87</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="198">
@@ -4092,10 +4101,10 @@
         <v>88</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="199">
@@ -4106,10 +4115,10 @@
         <v>89</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="200">
@@ -4120,10 +4129,10 @@
         <v>90</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="201">
@@ -4134,10 +4143,10 @@
         <v>91</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="202">
@@ -4148,10 +4157,10 @@
         <v>92</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="203">
@@ -4162,10 +4171,10 @@
         <v>93</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="204">
@@ -4176,10 +4185,10 @@
         <v>94</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="205">
@@ -4190,10 +4199,10 @@
         <v>95</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="206">
@@ -4204,10 +4213,10 @@
         <v>96</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="207">
@@ -4218,10 +4227,10 @@
         <v>97</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="208">
@@ -4232,10 +4241,10 @@
         <v>98</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D208" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="209">
@@ -4246,2404 +4255,2404 @@
         <v>99</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B210" s="0">
         <v>0</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B211" s="0">
         <v>1</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B212" s="0">
         <v>2</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B213" s="0">
         <v>3</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B214" s="0">
         <v>4</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B215" s="0">
         <v>5</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B216" s="0">
         <v>6</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B217" s="0">
         <v>7</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B218" s="0">
         <v>8</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B219" s="0">
         <v>9</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B220" s="0">
         <v>10</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B221" s="0">
         <v>11</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B222" s="0">
         <v>12</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B223" s="0">
         <v>13</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B224" s="0">
         <v>14</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B225" s="0">
         <v>15</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B226" s="0">
         <v>16</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B227" s="0">
         <v>17</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D227" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B228" s="0">
         <v>18</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D228" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B229" s="0">
         <v>19</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D229" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B230" s="0">
         <v>20</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D230" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B231" s="0">
         <v>21</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D231" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B232" s="0">
         <v>22</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D232" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B233" s="0">
         <v>23</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D233" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B234" s="0">
         <v>24</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D234" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B235" s="0">
         <v>25</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D235" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B236" s="0">
         <v>26</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D236" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B237" s="0">
         <v>27</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D237" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B238" s="0">
         <v>28</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D238" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B239" s="0">
         <v>29</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D239" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B240" s="0">
         <v>30</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D240" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B241" s="0">
         <v>31</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D241" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B242" s="0">
         <v>32</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D242" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B243" s="0">
         <v>33</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D243" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B244" s="0">
         <v>34</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D244" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B245" s="0">
         <v>35</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D245" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B246" s="0">
         <v>36</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D246" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B247" s="0">
         <v>37</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D247" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B248" s="0">
         <v>38</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D248" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B249" s="0">
         <v>39</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D249" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B250" s="0">
         <v>40</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D250" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B251" s="0">
         <v>41</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D251" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B252" s="0">
         <v>42</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D252" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B253" s="0">
         <v>43</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D253" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B254" s="0">
         <v>44</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D254" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B255" s="0">
         <v>45</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D255" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B256" s="0">
         <v>46</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D256" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B257" s="0">
         <v>47</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D257" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B258" s="0">
         <v>48</v>
       </c>
       <c r="C258" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D258" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B259" s="0">
         <v>49</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D259" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B260" s="0">
         <v>50</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D260" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B261" s="0">
         <v>51</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D261" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B262" s="0">
         <v>52</v>
       </c>
       <c r="C262" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D262" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B263" s="0">
         <v>53</v>
       </c>
       <c r="C263" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D263" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B264" s="0">
         <v>54</v>
       </c>
       <c r="C264" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D264" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B265" s="0">
         <v>55</v>
       </c>
       <c r="C265" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D265" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B266" s="0">
         <v>56</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D266" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B267" s="0">
         <v>57</v>
       </c>
       <c r="C267" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D267" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B268" s="0">
         <v>58</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D268" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B269" s="0">
         <v>59</v>
       </c>
       <c r="C269" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D269" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B270" s="0">
         <v>60</v>
       </c>
       <c r="C270" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D270" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B271" s="0">
         <v>61</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D271" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B272" s="0">
         <v>62</v>
       </c>
       <c r="C272" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D272" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B273" s="0">
         <v>63</v>
       </c>
       <c r="C273" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D273" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B274" s="0">
         <v>64</v>
       </c>
       <c r="C274" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D274" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B275" s="0">
         <v>65</v>
       </c>
       <c r="C275" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D275" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B276" s="0">
         <v>66</v>
       </c>
       <c r="C276" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D276" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B277" s="0">
         <v>67</v>
       </c>
       <c r="C277" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D277" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B278" s="0">
         <v>68</v>
       </c>
       <c r="C278" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D278" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B279" s="0">
         <v>69</v>
       </c>
       <c r="C279" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D279" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B280" s="0">
         <v>70</v>
       </c>
       <c r="C280" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D280" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B281" s="0">
         <v>71</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D281" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B282" s="0">
         <v>72</v>
       </c>
       <c r="C282" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D282" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B283" s="0">
         <v>73</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D283" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B284" s="0">
         <v>74</v>
       </c>
       <c r="C284" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D284" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B285" s="0">
         <v>75</v>
       </c>
       <c r="C285" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D285" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B286" s="0">
         <v>76</v>
       </c>
       <c r="C286" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D286" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B287" s="0">
         <v>77</v>
       </c>
       <c r="C287" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D287" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B288" s="0">
         <v>78</v>
       </c>
       <c r="C288" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D288" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B289" s="0">
         <v>79</v>
       </c>
       <c r="C289" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D289" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B290" s="0">
         <v>80</v>
       </c>
       <c r="C290" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D290" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B291" s="0">
         <v>81</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B292" s="0">
         <v>82</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D292" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B293" s="0">
         <v>83</v>
       </c>
       <c r="C293" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D293" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B294" s="0">
         <v>84</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D294" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B295" s="0">
         <v>85</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D295" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B296" s="0">
         <v>86</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B297" s="0">
         <v>87</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B298" s="0">
         <v>88</v>
       </c>
       <c r="C298" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D298" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B299" s="0">
         <v>89</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D299" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B300" s="0">
         <v>90</v>
       </c>
       <c r="C300" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D300" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B301" s="0">
         <v>91</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B302" s="0">
         <v>92</v>
       </c>
       <c r="C302" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D302" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B303" s="0">
         <v>93</v>
       </c>
       <c r="C303" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D303" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B304" s="0">
         <v>94</v>
       </c>
       <c r="C304" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D304" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B305" s="0">
         <v>95</v>
       </c>
       <c r="C305" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D305" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B306" s="0">
         <v>96</v>
       </c>
       <c r="C306" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D306" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B307" s="0">
         <v>97</v>
       </c>
       <c r="C307" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D307" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B308" s="0">
         <v>98</v>
       </c>
       <c r="C308" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D308" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B309" s="0">
         <v>99</v>
       </c>
       <c r="C309" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D309" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B310" s="0">
         <v>0</v>
       </c>
       <c r="C310" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D310" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B311" s="0">
         <v>1</v>
       </c>
       <c r="C311" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B312" s="0">
         <v>0</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D312" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B313" s="0">
         <v>1</v>
       </c>
       <c r="C313" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D313" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B314" s="0">
         <v>0</v>
       </c>
       <c r="C314" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D314" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B315" s="0">
         <v>1</v>
       </c>
       <c r="C315" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D315" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B316" s="0">
         <v>2</v>
       </c>
       <c r="C316" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D316" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B317" s="0">
         <v>0</v>
       </c>
       <c r="C317" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B318" s="0">
         <v>1</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D318" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B319" s="0">
         <v>0</v>
       </c>
       <c r="C319" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D319" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B320" s="0">
         <v>0</v>
       </c>
       <c r="C320" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D320" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B321" s="0">
         <v>1</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B322" s="0">
         <v>2</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D322" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B323" s="0">
         <v>3</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="D323" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B324" s="0">
         <v>4</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D324" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B325" s="0">
         <v>5</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D325" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B326" s="0">
         <v>6</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="D326" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B327" s="0">
         <v>7</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="D327" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B328" s="0">
         <v>8</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D328" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B329" s="0">
         <v>9</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D329" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B330" s="0">
         <v>10</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D330" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B331" s="0">
         <v>11</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D331" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B332" s="0">
         <v>12</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="D332" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B333" s="0">
         <v>13</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D333" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B334" s="0">
         <v>14</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D334" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B335" s="0">
         <v>15</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B336" s="0">
         <v>16</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D336" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B337" s="0">
         <v>17</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="D337" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B338" s="0">
         <v>18</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D338" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B339" s="0">
         <v>19</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D339" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B340" s="0">
         <v>20</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D340" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B341" s="0">
         <v>21</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D341" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B342" s="0">
         <v>22</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="D342" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B343" s="0">
         <v>23</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="D343" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B344" s="0">
         <v>24</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D344" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B345" s="0">
         <v>25</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D345" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B346" s="0">
         <v>26</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D346" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B347" s="0">
         <v>27</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="D347" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B348" s="0">
         <v>28</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D348" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B349" s="0">
         <v>29</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B350" s="0">
         <v>30</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B351" s="0">
         <v>31</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D351" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B352" s="0">
         <v>32</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="D352" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B353" s="0">
         <v>33</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="D353" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B354" s="0">
         <v>34</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D354" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B355" s="0">
         <v>35</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D355" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B356" s="0">
         <v>36</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="D356" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B357" s="0">
         <v>37</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="D357" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B358" s="0">
         <v>38</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B359" s="0">
         <v>39</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="D359" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B360" s="0">
         <v>40</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="D360" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B361" s="0">
         <v>41</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B362" s="0">
         <v>42</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="D362" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B363" s="0">
         <v>43</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D363" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B364" s="0">
         <v>44</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D364" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B365" s="0">
         <v>45</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="D365" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B366" s="0">
         <v>46</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="D366" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B367" s="0">
         <v>47</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="D367" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B368" s="0">
         <v>48</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B369" s="0">
         <v>49</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="D369" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B370" s="0">
         <v>50</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D370" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B371" s="0">
         <v>51</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="D371" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B372" s="0">
         <v>52</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B373" s="0">
         <v>53</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="D373" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B374" s="0">
         <v>54</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D374" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B375" s="0">
         <v>0</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D375" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B376" s="0">
         <v>0</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D376" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B377" s="0">
         <v>0</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D377" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B378" s="0">
         <v>1</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D378" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B379" s="0">
         <v>0</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D379" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B380" s="0">
         <v>1</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D380" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>